<commit_message>
case18_1, case18_2, case18_3. 2020 and 2025. RES added.
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
+++ b/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D111118-DF3A-46BE-A2A6-2DCA902FA34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E0F5BB-019E-4B62-BF60-98BFB9F58C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28215" yWindow="3615" windowWidth="21600" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26865" yWindow="3390" windowWidth="21600" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -8898,7 +8898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -8967,7 +8967,7 @@
       </c>
       <c r="B7" s="4">
         <f>SUM('RES installed'!$C$2:$C$7)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7442622950819669E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0140196885190942E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,55 +13510,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6618032363396047E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.32911444893864367</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.8555189821922381</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1801322843705835</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2899977247566496</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2121877958814882</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.95916766499098838</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.48059138405160062</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.11152136270159345</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.1026581196581302E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2624689390952954E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.1675048002194387E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,99 +13583,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.9969194904656238</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.6409570222502401</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.783116607383302</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.7074410111066287</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2499070939836967</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1112102266546926</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8186056900489413</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6328280054754465</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.598617998762335</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4451173907561699</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5223828904064418</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.430325650729233</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.406897906466007</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3596077484726243</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6453161396443827</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9622518161894376</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9725878024728962</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.269977836904399</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9939091355001093</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2084099750182382</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2568324538392486</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1568850287215184</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2190691637693529</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.5325362144333368</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.9938524590163926E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.070098442595471E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,55 +13712,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.0546585434827789E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43199473358221924</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.57871871637403605</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.64310900548742567</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.58300460659062048</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.46588143728133719</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.26011389342999003</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.1933967924761654E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.6568140814081463E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.2510597955203957E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6160738776629788E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,11 +13789,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.8121584699453533E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.0546585434827789E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.17148594971013539</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.42775949109611905</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.57304500346840825</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.66396941715415791</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.57145996091555862</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43390918178163751</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.2378184168502766</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.4120661311067408E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.0059201956960658E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5837524001097193E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.4882508914693243E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,55 +13914,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.6481596993183522E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.4108185211517183</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55602386475152488</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65132238063693582</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.63647901574013255</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55991531524049687</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.24029569202580031</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.4120661311067408E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.4106823643902904E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.8220654958278186E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6645560939928683E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8896174863387977E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0244734997409405E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,55 +14184,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6618032363396047E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.33950753679986401</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.80469607235903584</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1801322843705835</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2647036517222054</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2729580314802651</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1775538588563026</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.93176287456267437</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.49050048475369551</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.10605462923582906</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.3839515105356807E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2011840391392132E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.3291121879857366E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,99 +14257,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.9663386793384232</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.7521552126607762</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.8104020643184322</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.5980494551023203</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2972735591201952</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9857917973484729</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.855345198938819</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7317872785345645</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5663226856560251</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4893556782282973</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4063918130421413</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5025643199579823</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3392585840397564</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2929603098220055</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6117382592434768</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8314350284434751</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8554043686626251</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1835024907366121</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0144648997836154</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0191176914452464</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1683292203553566</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2022931345893397</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1092142546718602</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.383563495937258</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>9.0846994535519115E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,55 +14386,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.2242303022929415E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.16802158708972861</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43199473358221924</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56169757765715267</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.64499886237832482</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.68951893371847706</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55991531524049687</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.45674650713856585</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.24525024237684775</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.6854028043949602E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.9446352957399832E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5352701837798298E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>9.3572404371584697E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,55 +14487,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.7329455787234344E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.17495031233054217</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43199473358221924</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56737129056278046</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.66962896447659781</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.54837066956543501</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.25268206790341891</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.3027314617914531E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.4458440382499839E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.2510597955203957E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6483953552162382E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.6304644808743156E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.965560330377007E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,55 +14588,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.6481596993183522E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.57871871637403605</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.60073423456804753</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.63647901574013255</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.44304411192440885</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.2378184168502766</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.3403590166709027E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.1284899956082304E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5837524001097193E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0558349334064794E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,55 +14858,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7296319398636704E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.32911444893864367</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.8555189821922381</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1914797101818391</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3026447612738716</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3127379699640236</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.166009213181241</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.90435808413436036</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.48059138405160062</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.10714797592898194</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.7510413810611936E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2502119591040791E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.2321477553259576E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,99 +14931,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.0886619238472246</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.9189524982765813</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.6194038657725196</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.8715283451130915</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2499070939836967</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0694040835526191</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8002359356040025</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7317872785345645</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5501750291028702</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.400879103284042</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.449888467053754</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4736688522664827</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3392585840397564</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3995962116629956</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6285271994439297</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9061874785840249</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8944655132660486</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1618836541946655</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0144648997836154</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9980852154926918</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.3010840705811946</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2022931345893397</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1311852364913588</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.5325362144333368</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>9.4480874316939885E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.0178293864862386E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,55 +15060,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.902517337533597E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.17321813102033878</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43622997606831942</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.53900272603464139</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.66396941715415791</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.67625895422389093</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55414299240296594</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.46588143728133719</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.24029569202580031</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.3755206905305968E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.3736295954325596E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6483953552162382E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>9.5389344262295074E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.3314437231416288E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,55 +15161,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.3938020611031058E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.16802158708972861</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.42775949109611905</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.61970478934388062</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.59454925226568223</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.23534114167475287</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.4106823643902904E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.3123446954764769E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.680716832769498E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>9.1755464480874303E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.902517337533597E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.17321813102033878</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.44046521855441961</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56737129056278046</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.63867534411971372</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.69614892346577006</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.60609389794074409</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.43847664685302318</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.26011389342999003</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5999131388863491E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17000,7 +17000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303073B7-556E-4714-A27A-3E87EB1A31BB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -17025,7 +17025,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -17036,7 +17036,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -17047,7 +17047,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -17058,7 +17058,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -17069,7 +17069,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.3998142076502733E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3830392246502697E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,55 +26485,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0084706783250365E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.41968219233029214</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0786940747438072</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5115624164381969</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.614955400993271</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7011757445538596</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4156362222993999</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1941121649252506</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.6085498832872418</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.1333162551583334</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4586859467861387E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.8717897961049643E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,99 +26558,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.3818631724380968</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0349582676086979</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1098019869306546</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.072815503787508</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6874303204877728</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6334632820027528</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4125607684643824</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.31864288619348</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2087684054666183</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0785128851645276</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1315471534226982</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0392780687024945</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.94919901747301971</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.98240676699958296</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2934091816522886</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4507570978980424</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3340356397109177</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6019756234397571</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4485253921640393</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6375549601285497</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6941943539567657</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7130787966298029</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.678998593600614</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9004987356703438</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1191441256830601E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.3883240376702929E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,55 +26687,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0993734239252833E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.22077031992374743</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.69764419220224472</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.76750355690769312</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.84216621017517801</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56261053924362769</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.30737978798692317</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.9435549561631976E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.8197597147298159E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9358948980524821E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1191441256830601E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.6517600804608211E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,55 +26788,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.21202694091686636</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.79148804306105858</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.80847956176817082</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.5798333108531265</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.29496040261371415</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.0824260552864615E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.4438097284447284E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.857676922373594E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1076065573770491E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,55 +26889,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.21858447517202717</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.74124695421488507</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.86743119648043332</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.70781811114969995</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.60279700633245825</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.3042749416436209</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.0824260552864615E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.3024516946807136E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8772314162933162E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1921379781420765E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.290836609673585E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,55 +27240,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1987468478505665E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.45028401885437597</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4243568924129162</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.56698642868654</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7180190687573631</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4451286435973041</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.159666621706253</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.62096926866045088</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.13748238813203131</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4436479473347352E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>3.715353844747188E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,99 +27313,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2911255277737883</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.094809981361895</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0262454725967673</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9923178143200322</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7762424426187082</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5224512142938278</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3697558966927346</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3442476024302468</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1969177348247888</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1003010242587605</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0538919566191796</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0821348962778552</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0091484291028947</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.96215095737072553</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2809725549056319</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3810091604990982</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3340356397109177</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6019756234397571</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5692358415110428</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4958434731943482</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6941943539567657</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7466685769558774</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6954593641261104</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9191310762161315</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,11 +27418,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.130681693989071E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.3883240376702929E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,55 +27442,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0042353391625182E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.21202694091686636</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.69764419220224472</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.83146218665000093</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.84216621017517801</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.75205674309655623</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.57409238698329357</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.31048463433022544</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.7352483074783018E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.2585491263676448E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.7445697174727984E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8967859102130381E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1537568306010929E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,55 +27543,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0465189323904138E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.51237968550330837</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.71944557320856484</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.8169012238699227</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.70044500582522395</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.59131515859279238</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.30117009530031869</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.0129905057248296E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.4438097284447284E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9750038858919265E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.6517600804608211E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,55 +27644,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0888025256183095E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.74124695421488507</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.80747770049663548</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.86743119648043332</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.75205674309655623</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.58557423472295944</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.31048463433022544</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.0824260552864615E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.4341593996199193E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.7445697174727984E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0141128737313706E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1921379781420765E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3040084118131113E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,55 +27914,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0718960681668799E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.41968219233029214</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1326287784809976</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5260966704424104</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.646934715864425</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7180190687573631</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4598748542462563</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1826303171855848</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.65201773209347347</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.13748238813203131</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>8.5170982527352896E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.4286099478833317E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.1064437231416293E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,99 +27987,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.2911255277737883</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.975106553855501</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.1306911155141264</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.931944547219425</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7229551693401468</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5541689479249494</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.355487606102185</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3314452443118636</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1613657228993</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.111195093805877</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0760791557058991</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1142775169593757</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0091484291028947</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0026625766284405</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.1814795409323788</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3391603980597313</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.3480781201289271</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5702533338666924</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5390582291742918</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.5115891939648149</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.7114820514461202</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6123094556515791</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.6131555114986291</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9563957573077071</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,55 +28116,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.53934703737190359</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.75578120821909844</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.81547252921442404</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.88427452068393697</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.72256432179865204</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.55686961537379476</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.2212971544097254E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.7445697174727984E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.8967859102130381E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.130681693989071E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,55 +28217,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0148062374694922E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.21421278566858662</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56092091886677975</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.76304833522120519</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.80747770049663548</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.8169012238699227</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.58557423472295944</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.30117009530031869</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.6658127579166698E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.2585491263676448E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.142219262295082E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>6.7176190911584525E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,55 +28318,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.21639863042030691</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.54474050774562266</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.77549838562548157</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.74468363777208013</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.56835146311346063</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.0129905057248296E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>7.8949497119868334E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0</v>
+        <v>2.0336673676510925E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>

<commit_message>
DN node 5. RES updated
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
+++ b/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E0F5BB-019E-4B62-BF60-98BFB9F58C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10009F75-6278-4274-A370-9F222E5B93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26865" yWindow="3390" windowWidth="21600" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8355" yWindow="4620" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -8898,7 +8898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7442622950819669E-5</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0140196885190942E-5</v>
+        <v>1.0767425558501721E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13514,51 +13514,51 @@
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32911444893864367</v>
+        <v>0.35336498728149113</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8555189821922381</v>
+        <v>0.83010752727563697</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1687848585593277</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2899977247566496</v>
+        <v>1.2647036517222054</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3259979494586096</v>
+        <v>1.2596980519856791</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2121877958814882</v>
+        <v>1.1890985045313645</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95916766499098838</v>
+        <v>0.9134930142771317</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11152136270159345</v>
+        <v>0.10933466931528769</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1026581196581302E-4</v>
+        <v>6.7510413810611936E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2624689390952954E-4</v>
+        <v>1.1766700791567802E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1675048002194387E-5</v>
+        <v>3.361433665538996E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,35 +13583,35 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9969194904656238</v>
+        <v>3.1192427349744243</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6409570222502401</v>
+        <v>2.9189524982765813</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.783116607383302</v>
+        <v>2.592118408837389</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7074410111066287</v>
+        <v>2.6800931221055517</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2499070939836967</v>
+        <v>2.4156897219614426</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1112102266546926</v>
+        <v>2.1321132982057289</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8186056900489413</v>
+        <v>1.9288242167185743</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6328280054754465</v>
+        <v>1.7317872785345645</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13619,63 +13619,63 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4451173907561699</v>
+        <v>1.5335939657004252</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5223828904064418</v>
+        <v>1.4643873517242918</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.430325650729233</v>
+        <v>1.4592211184207329</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.406897906466007</v>
+        <v>1.2851471260987561</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3596077484726243</v>
+        <v>1.2796308220918817</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6453161396443827</v>
+        <v>1.6956829602457413</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9622518161894376</v>
+        <v>1.7940588033731999</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9725878024728962</v>
+        <v>1.9139960855677607</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.269977836904399</v>
+        <v>2.1618836541946655</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9939091355001093</v>
+        <v>1.9527976069330966</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2084099750182382</v>
+        <v>2.1242800712080196</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2568324538392486</v>
+        <v>2.1019517952424369</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1568850287215184</v>
+        <v>2.2022931345893397</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2190691637693529</v>
+        <v>2.3069530910473475</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5325362144333368</v>
+        <v>2.5821937872653633</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9938524590163926E-6</v>
+        <v>9.1755464480874303E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.070098442595471E-6</v>
+        <v>5.1746365548139341E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,55 +13712,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.0546585434827789E-3</v>
+        <v>8.5633738199132701E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16455722446932183</v>
+        <v>0.17841467495094895</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43199473358221924</v>
+        <v>0.43622997606831942</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57871871637403605</v>
+        <v>0.53900272603464139</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65764589889554681</v>
+        <v>0.64499886237832482</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64310900548742567</v>
+        <v>0.69614892346577006</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58300460659062048</v>
+        <v>0.54837066956543501</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.46588143728133719</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.25763661825446632</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1933967924761654E-2</v>
+        <v>5.4120661311067408E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6568140814081463E-4</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>5.8220654958278186E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6160738776629788E-5</v>
+        <v>1.5999131388863491E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13793,7 +13793,7 @@
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1223674987047025E-6</v>
+        <v>5.3837127792508603E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.0546585434827789E-3</v>
+        <v>8.3090161816980236E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17148594971013539</v>
+        <v>0.18187903757135573</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42775949109611905</v>
+        <v>0.41928900612391867</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57304500346840825</v>
+        <v>0.57871871637403605</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66396941715415791</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.64310900548742567</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57145996091555862</v>
+        <v>0.54837066956543501</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43390918178163751</v>
+        <v>0.47044890235272285</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2378184168502766</v>
+        <v>0.24525024237684775</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4120661311067408E-2</v>
+        <v>5.357398796449097E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5513290598290651E-4</v>
+        <v>3.3403590166709027E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.0059201956960658E-5</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5837524001097193E-5</v>
+        <v>1.6483953552162382E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7213114754098344E-6</v>
+        <v>8.6304644808743156E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4882508914693243E-6</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13918,35 +13918,35 @@
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16455722446932183</v>
+        <v>0.17321813102033878</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4108185211517183</v>
+        <v>0.43622997606831942</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55602386475152488</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65132238063693582</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63647901574013255</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55991531524049687</v>
+        <v>0.60609389794074409</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.47958383249549419</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24029569202580031</v>
+        <v>0.24772751755237146</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13954,15 +13954,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4106823643902904E-4</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8220654958278186E-5</v>
+        <v>6.189774895564313E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6645560939928683E-5</v>
+        <v>1.680716832769498E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8896174863387977E-5</v>
+        <v>1.7260928961748631E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0244734997409405E-5</v>
+        <v>1.0976501782938649E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,7 +14184,7 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6618032363396047E-2</v>
+        <v>1.7465891157446869E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14192,43 +14192,43 @@
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80469607235903584</v>
+        <v>0.8894009220810396</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1007003036917942</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2647036517222054</v>
+        <v>1.2141155056533173</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2729580314802651</v>
+        <v>1.2862180109748513</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1775538588563026</v>
+        <v>1.1082859848059319</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.93176287456267437</v>
+        <v>0.95003273484821704</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49050048475369551</v>
+        <v>0.5004095854557904</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.10386793584952331</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3839515105356807E-4</v>
+        <v>6.962011424219356E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2011840391392132E-4</v>
+        <v>1.1889270591479966E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,19 +14257,19 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9663386793384232</v>
+        <v>2.9357578682112226</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7521552126607762</v>
+        <v>2.8911529506739471</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8104020643184322</v>
+        <v>2.7285456935130408</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5980494551023203</v>
+        <v>2.7894846781098597</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14277,23 +14277,23 @@
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9857917973484729</v>
+        <v>2.1948225128588388</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.855345198938819</v>
+        <v>1.8186056900489413</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7317872785345645</v>
+        <v>1.6493212176519663</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5663226856560251</v>
+        <v>1.598617998762335</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4893556782282973</v>
+        <v>1.4746095824042549</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14301,55 +14301,55 @@
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5025643199579823</v>
+        <v>1.4447733845749831</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3392585840397564</v>
+        <v>1.3122028550692564</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2929603098220055</v>
+        <v>1.3462782607425006</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6117382592434768</v>
+        <v>1.7628387210475529</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8314350284434751</v>
+        <v>1.8501231409786123</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8554043686626251</v>
+        <v>1.9921183747746078</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1835024907366121</v>
+        <v>2.2267401638205051</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0144648997836154</v>
+        <v>1.9527976069330966</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0191176914452464</v>
+        <v>2.2084099750182382</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1683292203553566</v>
+        <v>2.1904550287263294</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2022931345893397</v>
+        <v>2.2477012404571615</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1092142546718602</v>
+        <v>2.2410401455888516</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.383563495937258</v>
+        <v>2.4580498551852976</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0846994535519115E-6</v>
+        <v>9.1755464480874303E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,11 +14386,11 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.2242303022929415E-3</v>
+        <v>8.3938020611031058E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16802158708972861</v>
+        <v>0.17495031233054217</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14398,43 +14398,43 @@
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56169757765715267</v>
+        <v>0.59006614218529174</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64499886237832482</v>
+        <v>0.60705775282665864</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68951893371847706</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55991531524049687</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45674650713856585</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24525024237684775</v>
+        <v>0.2502047927278952</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6854028043949602E-2</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.481005712109678E-4</v>
+        <v>3.5864907336887592E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.9446352957399832E-5</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5352701837798298E-5</v>
+        <v>1.6645560939928683E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14467,7 +14467,7 @@
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>4.965560330377007E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14491,19 +14491,19 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17495031233054217</v>
+        <v>0.18014685626115234</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43199473358221924</v>
+        <v>0.41928900612391867</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56737129056278046</v>
+        <v>0.58439242927966384</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65764589889554681</v>
+        <v>0.63235182586110272</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14511,31 +14511,31 @@
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54837066956543501</v>
+        <v>0.57145996091555862</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.45674650713856585</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25268206790341891</v>
+        <v>0.23534114167475287</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3027314617914531E-2</v>
+        <v>5.6854028043949602E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4458440382499839E-4</v>
+        <v>3.6919757552678404E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.6968775715461277E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14568,7 +14568,7 @@
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.965560330377007E-6</v>
+        <v>5.3837127792508603E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,43 +14588,43 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6481596993183522E-3</v>
+        <v>8.7329455787234344E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16628940577952522</v>
+        <v>0.18014685626115234</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.43622997606831942</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57871871637403605</v>
+        <v>0.57304500346840825</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60073423456804753</v>
+        <v>0.64499886237832482</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63647901574013255</v>
+        <v>0.62984902599283954</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60032157510321316</v>
+        <v>0.57145996091555862</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44304411192440885</v>
+        <v>0.47958383249549419</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2378184168502766</v>
+        <v>0.24277296720132402</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5760681350796724E-2</v>
+        <v>5.1933967924761654E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14632,11 +14632,11 @@
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.1284899956082304E-5</v>
+        <v>5.8833503957839012E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5837524001097193E-5</v>
+        <v>1.6483953552162382E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8351092896174861E-5</v>
+        <v>1.8896174863387977E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0558349334064794E-5</v>
+        <v>1.0453811221846331E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,39 +14858,39 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7296319398636704E-2</v>
+        <v>1.712674763982654E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32911444893864367</v>
+        <v>0.35682934990189791</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8555189821922381</v>
+        <v>0.83010752727563697</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1914797101818391</v>
+        <v>1.1233951553143053</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3026447612738716</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3127379699640236</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.166009213181241</v>
+        <v>1.1198306304809937</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90435808413436036</v>
+        <v>0.88608822384881769</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.5004095854557904</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14898,15 +14898,15 @@
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7510413810611936E-4</v>
+        <v>7.0323347719387431E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2502119591040791E-4</v>
+        <v>1.1889270591479966E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2321477553259576E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,15 +14931,15 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0886619238472246</v>
+        <v>2.9969194904656238</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9189524982765813</v>
+        <v>2.6687565698528743</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6194038657725196</v>
+        <v>2.783116607383302</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14947,19 +14947,19 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2499070939836967</v>
+        <v>2.3683232568249437</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0694040835526191</v>
+        <v>2.1739194413078025</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8002359356040025</v>
+        <v>1.9288242167185743</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7317872785345645</v>
+        <v>1.5833483689458874</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14967,63 +14967,63 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.400879103284042</v>
+        <v>1.5483400615244678</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.449888467053754</v>
+        <v>1.4788862363948292</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4736688522664827</v>
+        <v>1.4447733845749831</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3392585840397564</v>
+        <v>1.3663143130102569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3995962116629956</v>
+        <v>1.3596077484726243</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6285271994439297</v>
+        <v>1.6956829602457413</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9061874785840249</v>
+        <v>1.8874993660488877</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8944655132660486</v>
+        <v>1.8554043686626251</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1618836541946655</v>
+        <v>2.1402648176527186</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0144648997836154</v>
+        <v>1.9527976069330966</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9980852154926918</v>
+        <v>2.0611826433503557</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3010840705811946</v>
+        <v>2.2347066454682754</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2022931345893397</v>
+        <v>2.2249971875232504</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1311852364913588</v>
+        <v>2.2849821092278488</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5325362144333368</v>
+        <v>2.6070225736813764</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.4480874316939885E-6</v>
+        <v>9.5389344262295074E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.0178293864862386E-6</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15064,47 +15064,47 @@
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17321813102033878</v>
+        <v>0.18187903757135573</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43622997606831942</v>
+        <v>0.4108185211517183</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53900272603464139</v>
+        <v>0.56737129056278046</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66396941715415791</v>
+        <v>0.60705775282665864</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.67625895422389093</v>
+        <v>0.66962896447659781</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55414299240296594</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.46588143728133719</v>
+        <v>0.46131397220995152</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24029569202580031</v>
+        <v>0.2378184168502766</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5214008004220286E-2</v>
+        <v>5.6307354697373163E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3755206905305968E-4</v>
+        <v>3.6919757552678404E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3736295954325596E-5</v>
+        <v>6.2510597955203957E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5389344262295074E-6</v>
+        <v>9.2663934426229492E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3314437231416288E-6</v>
+        <v>5.4359818353600928E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,55 +15161,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3938020611031058E-3</v>
+        <v>8.1394444228878593E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16802158708972861</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42775949109611905</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54467643894026918</v>
+        <v>0.56169757765715267</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61970478934388062</v>
+        <v>0.63867534411971372</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.62984902599283954</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59454925226568223</v>
+        <v>0.58300460659062048</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.44304411192440885</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23534114167475287</v>
+        <v>0.25763661825446632</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2480641271338092E-2</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4106823643902904E-4</v>
+        <v>3.5161673859693715E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3123446954764769E-5</v>
+        <v>5.9446352957399832E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.680716832769498E-5</v>
+        <v>1.6483953552162382E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.1755464480874303E-6</v>
+        <v>9.5389344262295074E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>5.3314437231416288E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.902517337533597E-3</v>
+        <v>8.3938020611031058E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17321813102033878</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44046521855441961</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56737129056278046</v>
+        <v>0.57304500346840825</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63867534411971372</v>
+        <v>0.60705775282665864</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69614892346577006</v>
+        <v>0.68951893371847706</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60609389794074409</v>
+        <v>0.55991531524049687</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43847664685302318</v>
+        <v>0.45674650713856585</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.24277296720132402</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5214008004220286E-2</v>
+        <v>5.6854028043949602E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5513290598290651E-4</v>
+        <v>3.6568140814081463E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4349144953886422E-5</v>
+        <v>6.2510597955203957E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5999131388863491E-5</v>
+        <v>1.5514309225564595E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17000,7 +17000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303073B7-556E-4714-A27A-3E87EB1A31BB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3998142076502733E-5</v>
+        <v>2.3536639344262295E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3830392246502697E-5</v>
+        <v>1.3040084118131113E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,19 +26485,19 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0084706783250365E-2</v>
+        <v>2.1353214580087234E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41968219233029214</v>
+        <v>0.42842557133717324</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0786940747438072</v>
+        <v>1.0894810154912453</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115624164381969</v>
+        <v>1.4243568924129162</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26505,35 +26505,35 @@
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7011757445538596</v>
+        <v>1.6674890961468525</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4156362222993999</v>
+        <v>1.4303824329483521</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1941121649252506</v>
+        <v>1.0907755352682578</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6085498832872418</v>
+        <v>0.62096926866045088</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1333162551583334</v>
+        <v>0.14164852110572923</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3414879794830156E-4</v>
+        <v>9.0439290724921126E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4586859467861387E-4</v>
+        <v>1.4887619456889457E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8717897961049643E-5</v>
+        <v>3.9891167596232968E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,99 +26558,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3818631724380968</v>
+        <v>2.3138099389398654</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0349582676086979</v>
+        <v>1.915254840102304</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1098019869306546</v>
+        <v>1.9844672154298235</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.072815503787508</v>
+        <v>2.1130643485212461</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6874303204877728</v>
+        <v>1.7940048670448951</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6334632820027528</v>
+        <v>1.5541689479249494</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4125607684643824</v>
+        <v>1.3840241872832837</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.31864288619348</v>
+        <v>1.2802358118383304</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2087684054666183</v>
+        <v>1.1258137109738111</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0785128851645276</v>
+        <v>1.0676188156174111</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1315471534226982</v>
+        <v>1.0538919566191796</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0392780687024945</v>
+        <v>1.0178496549148142</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94919901747301971</v>
+        <v>0.98916529189293634</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.98240676699958296</v>
+        <v>0.97227886218515425</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2934091816522886</v>
+        <v>1.1814795409323788</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4507570978980424</v>
+        <v>1.4368075104182534</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3340356397109177</v>
+        <v>1.3480781201289271</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6019756234397571</v>
+        <v>1.5385310442936277</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4485253921640393</v>
+        <v>1.4636141983324147</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6375549601285497</v>
+        <v>1.5745720770466822</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6941943539567657</v>
+        <v>1.6596189589780561</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7130787966298029</v>
+        <v>1.7634634671189149</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.678998593600614</v>
+        <v>1.7119201346516064</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9004987356703438</v>
+        <v>1.8446017140329807</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1191441256830601E-5</v>
+        <v>1.1883695355191256E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3883240376702929E-6</v>
+        <v>6.5859010697631888E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,39 +26687,39 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0993734239252833E-2</v>
+        <v>1.0465189323904138E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22077031992374743</v>
+        <v>0.22295616467546772</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55013397811934173</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69764419220224472</v>
+        <v>0.69037706520013797</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76750355690769312</v>
+        <v>0.80747770049663548</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84216621017517801</v>
+        <v>0.82532288597167447</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73731053244760414</v>
+        <v>0.72256432179865204</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56261053924362769</v>
+        <v>0.5798333108531265</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30737978798692317</v>
+        <v>0.30117009530031869</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26727,11 +26727,11 @@
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.3024516946807136E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.8197597147298159E-5</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1191441256830601E-5</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6517600804608211E-6</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,15 +26788,15 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.025377135776466E-2</v>
+        <v>1.0148062374694922E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21202694091686636</v>
+        <v>0.21639863042030691</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55013397811934173</v>
+        <v>0.53934703737190359</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26804,15 +26804,15 @@
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79148804306105858</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80847956176817082</v>
+        <v>0.84216621017517801</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76680295374550833</v>
+        <v>0.75942984842103223</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26820,23 +26820,23 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29496040261371415</v>
+        <v>0.29806524895701642</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0824260552864615E-2</v>
+        <v>7.0129905057248296E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1707439897415078E-4</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.8197597147298159E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.857676922373594E-5</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1076065573770491E-5</v>
+        <v>1.1191441256830601E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2566060162750292E-6</v>
+        <v>6.5200420590655566E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,23 +26889,23 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21858447517202717</v>
+        <v>0.21202694091686636</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55552744849306068</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74124695421488507</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.82346735793221248</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26913,31 +26913,31 @@
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70781811114969995</v>
+        <v>0.77417605906998432</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60279700633245825</v>
+        <v>0.56835146311346063</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3042749416436209</v>
+        <v>0.30117009530031869</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0824260552864615E-2</v>
+        <v>7.1518616048480935E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3024516946807136E-4</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2934297339306934E-5</v>
+        <v>7.3686197311877109E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>1.9163404041327603E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1921379781420765E-5</v>
+        <v>2.284438524590164E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.290836609673585E-5</v>
+        <v>1.3435238182316905E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,55 +27240,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1987468478505665E-2</v>
+        <v>2.0296124749389844E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45028401885437597</v>
+        <v>0.43279726084061382</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0247593710066167</v>
+        <v>1.0679071339963691</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4243568924129162</v>
+        <v>1.3952883844044894</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.56698642868654</v>
+        <v>1.5509967712509631</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7180190687573631</v>
+        <v>1.6674890961468525</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4451286435973041</v>
+        <v>1.4746210648952083</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.159666621706253</v>
+        <v>1.1711484694459189</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62096926866045088</v>
+        <v>0.64580803940686893</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13748238813203131</v>
+        <v>0.13470496614956604</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3414879794830156E-4</v>
+        <v>8.6049033893614271E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4436479473347352E-4</v>
+        <v>1.4737239462375422E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.715353844747188E-5</v>
+        <v>3.8717897961049643E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,7 +27313,7 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2911255277737883</v>
+        <v>2.3138099389398654</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27321,91 +27321,91 @@
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0262454725967673</v>
+        <v>2.1306911155141264</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9923178143200322</v>
+        <v>2.072815503787508</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7762424426187082</v>
+        <v>1.7584800181925211</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5224512142938278</v>
+        <v>1.6651810156338742</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3697558966927346</v>
+        <v>1.4696339308265798</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3442476024302468</v>
+        <v>1.2162240212464137</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1969177348247888</v>
+        <v>1.1376643816156409</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1003010242587605</v>
+        <v>1.0676188156174111</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0538919566191796</v>
+        <v>1.1648279520527773</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0821348962778552</v>
+        <v>1.071420689384015</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0091484291028947</v>
+        <v>0.95919058607799879</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.96215095737072553</v>
+        <v>1.0229183862572979</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2809725549056319</v>
+        <v>1.1939161676790355</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3810091604990982</v>
+        <v>1.394958747978887</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3340356397109177</v>
+        <v>1.390205561382956</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6019756234397571</v>
+        <v>1.5226698995070955</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5692358415110428</v>
+        <v>1.4937918106691654</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4958434731943482</v>
+        <v>1.5115891939648149</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6941943539567657</v>
+        <v>1.728769748935475</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7466685769558774</v>
+        <v>1.7298736867928401</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6954593641261104</v>
+        <v>1.5802339704476367</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9191310762161315</v>
+        <v>1.8259693734871931</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27422,7 +27422,7 @@
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3883240376702929E-6</v>
+        <v>6.3224650269726606E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,55 +27442,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0042353391625182E-2</v>
+        <v>1.0570898306973877E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21202694091686636</v>
+        <v>0.20765525141342581</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55552744849306068</v>
+        <v>0.53395356699818453</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69764419220224472</v>
+        <v>0.76304833522120519</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83146218665000093</v>
+        <v>0.82346735793221248</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84216621017517801</v>
+        <v>0.85900953437868155</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75205674309655623</v>
+        <v>0.71519121647417605</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57409238698329357</v>
+        <v>0.5798333108531265</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31048463433022544</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7352483074783018E-2</v>
+        <v>7.2212971544097254E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2585491263676448E-4</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7445697174727984E-5</v>
+        <v>7.4438097284447284E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8967859102130381E-5</v>
+        <v>1.8772314162933162E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1537568306010929E-5</v>
+        <v>1.1999071038251367E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.849337112553717E-6</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,19 +27543,19 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0465189323904138E-2</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22514200942718798</v>
+        <v>0.22077031992374743</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51237968550330837</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71944557320856484</v>
+        <v>0.73397982721277832</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27563,7 +27563,7 @@
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8169012238699227</v>
+        <v>0.83374454807342624</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27571,27 +27571,27 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59131515859279238</v>
+        <v>0.55112869150396182</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30117009530031869</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0129905057248296E-2</v>
+        <v>7.1518616048480935E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.4780619679329875E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.3686197311877109E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9750038858919265E-5</v>
+        <v>1.8772314162933162E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2114446721311475E-5</v>
+        <v>1.1076065573770491E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6517600804608211E-6</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,55 +27644,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0888025256183095E-2</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22514200942718798</v>
+        <v>0.22077031992374743</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51777315587702744</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74124695421488507</v>
+        <v>0.7485140812169917</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80747770049663548</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86743119648043332</v>
+        <v>0.85058787227692978</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75205674309655623</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58557423472295944</v>
+        <v>0.60279700633245825</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31048463433022544</v>
+        <v>0.29806524895701642</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0824260552864615E-2</v>
+        <v>6.7352483074783018E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4341593996199193E-4</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7445697174727984E-5</v>
+        <v>7.5189997257017459E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0141128737313706E-5</v>
+        <v>1.9358948980524821E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1921379781420765E-5</v>
+        <v>2.2382882513661202E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3040084118131113E-5</v>
+        <v>1.3171802139526378E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,43 +27914,43 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0718960681668799E-2</v>
+        <v>2.1353214580087234E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41968219233029214</v>
+        <v>0.45465570835781655</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1326287784809976</v>
+        <v>1.046333252501493</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5260966704424104</v>
+        <v>1.4243568924129162</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.646934715864425</v>
+        <v>1.6309450584288481</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7180190687573631</v>
+        <v>1.7685490413678739</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4598748542462563</v>
+        <v>1.4303824329483521</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1826303171855848</v>
+        <v>1.1941121649252506</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65201773209347347</v>
+        <v>0.64580803940686893</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13748238813203131</v>
+        <v>0.13192754416710076</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27958,11 +27958,11 @@
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4286099478833317E-4</v>
+        <v>1.5639519429459632E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1064437231416293E-5</v>
+        <v>3.9108987839444087E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,51 +27987,51 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2911255277737883</v>
+        <v>2.2003878831094799</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.975106553855501</v>
+        <v>1.915254840102304</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1306911155141264</v>
+        <v>2.0262454725967673</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.931944547219425</v>
+        <v>1.9118201248525559</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7229551693401468</v>
+        <v>1.7940048670448951</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5541689479249494</v>
+        <v>1.5224512142938278</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.355487606102185</v>
+        <v>1.3840241872832837</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3314452443118636</v>
+        <v>1.2930381699567137</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1613657228993</v>
+        <v>1.185067064182959</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.111195093805877</v>
+        <v>1.0349366069760619</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0760791557058991</v>
+        <v>1.0538919566191796</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1142775169593757</v>
+        <v>1.1035633100655355</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28039,7 +28039,7 @@
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0026625766284405</v>
+        <v>1.0533021007005841</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28047,39 +28047,39 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3391603980597313</v>
+        <v>1.394958747978887</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3480781201289271</v>
+        <v>1.3761630809649468</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5702533338666924</v>
+        <v>1.5861144786532246</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5390582291742918</v>
+        <v>1.4485253921640393</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115891939648149</v>
+        <v>1.6375549601285497</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7114820514461202</v>
+        <v>1.7633451439141845</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6123094556515791</v>
+        <v>1.6626941261406909</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6131555114986291</v>
+        <v>1.6625378230751178</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9563957573077071</v>
+        <v>1.9377634167619193</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2114446721311475E-5</v>
+        <v>1.1768319672131148E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2566060162750292E-6</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,55 +28116,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.03594803408344E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22514200942718798</v>
+        <v>0.21858447517202717</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53934703737190359</v>
+        <v>0.5231666262507465</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75578120821909844</v>
+        <v>0.69037706520013797</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81547252921442404</v>
+        <v>0.82346735793221248</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88427452068393697</v>
+        <v>0.83374454807342624</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72256432179865204</v>
+        <v>0.70044500582522395</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55686961537379476</v>
+        <v>0.55112869150396182</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31669432701682998</v>
+        <v>0.32600886604673673</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2212971544097254E-2</v>
+        <v>6.6658127579166698E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.5658671045591245E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7445697174727984E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8967859102130381E-5</v>
+        <v>1.9163404041327603E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.130681693989071E-5</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.5859010697631888E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28221,27 +28221,27 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21421278566858662</v>
+        <v>0.22077031992374743</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56092091886677975</v>
+        <v>0.53934703737190359</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76304833522120519</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80747770049663548</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8169012238699227</v>
+        <v>0.85900953437868155</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73731053244760414</v>
+        <v>0.77417605906998432</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28249,11 +28249,11 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30117009530031869</v>
+        <v>0.32290401970343446</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6658127579166698E-2</v>
+        <v>7.2907327039713574E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28261,11 +28261,11 @@
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2934297339306934E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9945583798116484E-5</v>
+        <v>2.0336673676510925E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.142219262295082E-5</v>
+        <v>1.1537568306010929E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7176190911584525E-6</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,23 +28318,23 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.0148062374694922E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21639863042030691</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54474050774562266</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72671270021067158</v>
+        <v>0.69037706520013797</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.77549838562548157</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28342,15 +28342,15 @@
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74468363777208013</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56835146311346063</v>
+        <v>0.54538776763412888</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31669432701682998</v>
+        <v>0.29496040261371415</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28358,15 +28358,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2146465580545766E-4</v>
+        <v>4.1707439897415078E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.8949497119868334E-5</v>
+        <v>7.5941897229587634E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0336673676510925E-5</v>
+        <v>2.0141128737313706E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>

<commit_message>
DNs. Load and FL updated.
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
+++ b/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10009F75-6278-4274-A370-9F222E5B93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56600F21-090D-44D3-8422-9DC383D50D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8355" yWindow="4620" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7724,18 +7724,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
       <sheetData sheetId="27">
         <row r="2">
           <cell r="B2">
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8351092896174861E-5</v>
+        <v>1.7260928961748631E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0767425558501721E-5</v>
+        <v>1.0349273109627868E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,11 +13510,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6618032363396047E-2</v>
+        <v>1.6448460604585883E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35336498728149113</v>
+        <v>0.35682934990189791</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13522,11 +13522,11 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1687848585593277</v>
+        <v>1.1233951553143053</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2647036517222054</v>
+        <v>1.2267625421705393</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13538,27 +13538,27 @@
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9134930142771317</v>
+        <v>0.93176287456267437</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49545503510474292</v>
+        <v>0.51031868615788523</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10933466931528769</v>
+        <v>0.11042801600844057</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7510413810611936E-4</v>
+        <v>6.6807180333418054E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1766700791567802E-4</v>
+        <v>1.2869828990777284E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.361433665538996E-5</v>
+        <v>3.2967907104324765E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,99 +13583,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1192427349744243</v>
+        <v>3.1804043572288254</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9189524982765813</v>
+        <v>2.8077543078660447</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.592118408837389</v>
+        <v>2.7285456935130408</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6800931221055517</v>
+        <v>2.6253973441033973</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4156897219614426</v>
+        <v>2.3209567916884448</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1321132982057289</v>
+        <v>2.1530163697567657</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9288242167185743</v>
+        <v>1.8002359356040025</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7317872785345645</v>
+        <v>1.5668551567693678</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.598617998762335</v>
+        <v>1.6793562815281096</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5335939657004252</v>
+        <v>1.5041017740523399</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4643873517242918</v>
+        <v>1.4788862363948292</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4592211184207329</v>
+        <v>1.5025643199579823</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2851471260987561</v>
+        <v>1.3257307195545065</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2796308220918817</v>
+        <v>1.3329487730123768</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6956829602457413</v>
+        <v>1.7460497808471001</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7940588033731999</v>
+        <v>1.9061874785840249</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9139960855677607</v>
+        <v>2.031179519378032</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1618836541946655</v>
+        <v>2.0754083080268786</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9527976069330966</v>
+        <v>1.9939091355001093</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1242800712080196</v>
+        <v>2.0822151193029104</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1019517952424369</v>
+        <v>2.1462034119843834</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2022931345893397</v>
+        <v>2.3839255580606258</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3069530910473475</v>
+        <v>2.2190691637693529</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5821937872653633</v>
+        <v>2.5325362144333368</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.1755464480874303E-6</v>
+        <v>9.0846994535519115E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1746365548139341E-6</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,19 +13712,19 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5633738199132701E-3</v>
+        <v>8.902517337533597E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17841467495094895</v>
+        <v>0.18187903757135573</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43622997606831942</v>
+        <v>0.4447004610405198</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53900272603464139</v>
+        <v>0.57871871637403605</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13732,27 +13732,27 @@
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69614892346577006</v>
+        <v>0.68951893371847706</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54837066956543501</v>
+        <v>0.5656876380780278</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.45217904206718018</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25763661825446632</v>
+        <v>0.25515934307894261</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4120661311067408E-2</v>
+        <v>5.4667334657643847E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5513290598290651E-4</v>
+        <v>3.6216524075484527E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13760,7 +13760,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5999131388863491E-5</v>
+        <v>1.6968775715461277E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13793,7 +13793,7 @@
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3837127792508603E-6</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3090161816980236E-3</v>
+        <v>8.2242303022929415E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.18187903757135573</v>
+        <v>0.17668249364074556</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41928900612391867</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57871871637403605</v>
+        <v>0.55035015184589708</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65764589889554681</v>
+        <v>0.61970478934388062</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64310900548742567</v>
+        <v>0.66962896447659781</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54837066956543501</v>
+        <v>0.57723228375308955</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47044890235272285</v>
+        <v>0.46131397220995152</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24525024237684775</v>
+        <v>0.25763661825446632</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.357398796449097E-2</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3403590166709027E-4</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4349144953886422E-5</v>
+        <v>6.3123446954764769E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.5675916613330893E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6304644808743156E-6</v>
+        <v>9.0846994535519115E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1223674987047025E-6</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,35 +13914,35 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6481596993183522E-3</v>
+        <v>8.902517337533597E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17321813102033878</v>
+        <v>0.17841467495094895</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43622997606831942</v>
+        <v>0.4447004610405198</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54467643894026918</v>
+        <v>0.55602386475152488</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65764589889554681</v>
+        <v>0.63867534411971372</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.64310900548742567</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60609389794074409</v>
+        <v>0.59454925226568223</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47958383249549419</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13950,19 +13950,19 @@
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4120661311067408E-2</v>
+        <v>5.6307354697373163E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5513290598290651E-4</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.189774895564313E-5</v>
+        <v>6.0672050956521478E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.680716832769498E-5</v>
+        <v>1.5837524001097193E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14164,7 +14164,7 @@
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0976501782938649E-5</v>
+        <v>1.0349273109627868E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,19 +14184,19 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7465891157446869E-2</v>
+        <v>1.7296319398636704E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.34643626204067757</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8894009220810396</v>
+        <v>0.81316655733123622</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1007003036917942</v>
+        <v>1.1120477295030498</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14204,35 +14204,35 @@
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2862180109748513</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1082859848059319</v>
+        <v>1.1429199218311172</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95003273484821704</v>
+        <v>0.88608822384881769</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5004095854557904</v>
+        <v>0.48059138405160062</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10386793584952331</v>
+        <v>0.10824132262213482</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.962011424219356E-4</v>
+        <v>7.2433048150969054E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1889270591479966E-4</v>
+        <v>1.2379549791128626E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3291121879857366E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,95 +14257,95 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9357578682112226</v>
+        <v>2.905177057084023</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8911529506739471</v>
+        <v>2.8077543078660447</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7285456935130408</v>
+        <v>2.8376875212535624</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7894846781098597</v>
+        <v>2.8168325671109375</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2972735591201952</v>
+        <v>2.4393729545296923</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1948225128588388</v>
+        <v>2.1321132982057289</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8186056900489413</v>
+        <v>1.855345198938819</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6493212176519663</v>
+        <v>1.5668551567693678</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.598617998762335</v>
+        <v>1.6470609684217996</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4746095824042549</v>
+        <v>1.5041017740523399</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4063918130421413</v>
+        <v>1.5078840057359042</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4447733845749831</v>
+        <v>1.3725347153462339</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3122028550692564</v>
+        <v>1.406897906466007</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3462782607425006</v>
+        <v>1.266301334361758</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7628387210475529</v>
+        <v>1.6285271994439297</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8501231409786123</v>
+        <v>1.8874993660488877</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9921183747746078</v>
+        <v>1.9530572301711844</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2267401638205051</v>
+        <v>2.1186459811107721</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9527976069330966</v>
+        <v>2.0555764283506281</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2084099750182382</v>
+        <v>2.1663450231131289</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1904550287263294</v>
+        <v>2.1240776036134101</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2477012404571615</v>
+        <v>2.2249971875232504</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2410401455888516</v>
+        <v>2.2630111274083502</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.1755464480874303E-6</v>
+        <v>8.9938524590163926E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1223674987047025E-6</v>
+        <v>5.2269056109231657E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,7 +14386,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3938020611031058E-3</v>
+        <v>8.3090161816980236E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14394,47 +14394,47 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43199473358221924</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59006614218529174</v>
+        <v>0.55602386475152488</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60705775282665864</v>
+        <v>0.60073423456804753</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.67625895422389093</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60032157510321316</v>
+        <v>0.60609389794074409</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.44304411192440885</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2502047927278952</v>
+        <v>0.26011389342999003</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2480641271338092E-2</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5864907336887592E-4</v>
+        <v>3.4106823643902904E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4349144953886422E-5</v>
+        <v>6.2510597955203957E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6645560939928683E-5</v>
+        <v>1.5514309225564595E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.3572404371584697E-6</v>
+        <v>8.9938524590163926E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.965560330377007E-6</v>
+        <v>5.3314437231416288E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,51 +14487,51 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7329455787234344E-3</v>
+        <v>8.0546585434827789E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.18014685626115234</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41928900612391867</v>
+        <v>0.42352424861001886</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58439242927966384</v>
+        <v>0.59573985509091953</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63235182586110272</v>
+        <v>0.60073423456804753</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66962896447659781</v>
+        <v>0.62984902599283954</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57145996091555862</v>
+        <v>0.58300460659062048</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45674650713856585</v>
+        <v>0.44761157699579451</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.23534114167475287</v>
+        <v>0.2378184168502766</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6854028043949602E-2</v>
+        <v>5.2480641271338092E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6919757552678404E-4</v>
+        <v>3.4458440382499839E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4349144953886422E-5</v>
+        <v>5.8833503957839012E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6304644808743156E-6</v>
+        <v>9.5389344262295074E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3837127792508603E-6</v>
+        <v>5.4359818353600928E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,11 +14588,11 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7329455787234344E-3</v>
+        <v>8.3938020611031058E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.18014685626115234</v>
+        <v>0.169753768399932</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14600,23 +14600,23 @@
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57304500346840825</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64499886237832482</v>
+        <v>0.61970478934388062</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62984902599283954</v>
+        <v>0.6629989747293048</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57145996091555862</v>
+        <v>0.60609389794074409</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47958383249549419</v>
+        <v>0.43390918178163751</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14624,15 +14624,15 @@
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1933967924761654E-2</v>
+        <v>5.4120661311067408E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3403590166709027E-4</v>
+        <v>3.6919757552678404E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8833503957839012E-5</v>
+        <v>6.4349144953886422E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8896174863387977E-5</v>
+        <v>1.8532786885245898E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0453811221846331E-5</v>
+        <v>1.0035658772972477E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,55 +14858,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.712674763982654E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35682934990189791</v>
+        <v>0.32911444893864367</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83010752727563697</v>
+        <v>0.8555189821922381</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1233951553143053</v>
+        <v>1.1574374327480721</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2394095786877612</v>
+        <v>1.2647036517222054</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3259979494586096</v>
+        <v>1.2862180109748513</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1198306304809937</v>
+        <v>1.09674133913087</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88608822384881769</v>
+        <v>0.95916766499098838</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5004095854557904</v>
+        <v>0.47563683370055321</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10714797592898194</v>
+        <v>0.11152136270159345</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0323347719387431E-4</v>
+        <v>7.3136281628162925E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1889270591479966E-4</v>
+        <v>1.2624689390952954E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3937551430922555E-5</v>
+        <v>3.0705403675596596E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,11 +14931,11 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9969194904656238</v>
+        <v>2.9357578682112226</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6687565698528743</v>
+        <v>2.8911529506739471</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14943,11 +14943,11 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8715283451130915</v>
+        <v>2.7347889001077057</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3683232568249437</v>
+        <v>2.3209567916884448</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14959,7 +14959,7 @@
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5833483689458874</v>
+        <v>1.6328280054754465</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14967,35 +14967,35 @@
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5483400615244678</v>
+        <v>1.430371294932127</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4788862363948292</v>
+        <v>1.449888467053754</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4447733845749831</v>
+        <v>1.430325650729233</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3663143130102569</v>
+        <v>1.4204257709512569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3596077484726243</v>
+        <v>1.3862667239328719</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6956829602457413</v>
+        <v>1.7124719004461941</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8874993660488877</v>
+        <v>1.7753706908380624</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8554043686626251</v>
+        <v>2.0116489470763197</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15003,27 +15003,27 @@
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9527976069330966</v>
+        <v>2.0966879569176409</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0611826433503557</v>
+        <v>2.0822151193029104</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2347066454682754</v>
+        <v>2.1683292203553566</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2249971875232504</v>
+        <v>2.3385174521928045</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2849821092278488</v>
+        <v>2.1092142546718602</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6070225736813764</v>
+        <v>2.4580498551852976</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,7 +15036,7 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5389344262295074E-6</v>
+        <v>9.1755464480874303E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,47 +15060,47 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.902517337533597E-3</v>
+        <v>8.0546585434827789E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.18187903757135573</v>
+        <v>0.17148594971013539</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4108185211517183</v>
+        <v>0.41505376363781848</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56737129056278046</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60705775282665864</v>
+        <v>0.61338127108526963</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66962896447659781</v>
+        <v>0.62984902599283954</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60032157510321316</v>
+        <v>0.57723228375308955</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.46131397220995152</v>
+        <v>0.47501636742410852</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2378184168502766</v>
+        <v>0.24277296720132402</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6307354697373163E-2</v>
+        <v>5.6854028043949602E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6919757552678404E-4</v>
+        <v>3.5161673859693715E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15108,7 +15108,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.5352701837798298E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.2663934426229492E-6</v>
+        <v>8.9030054644808738E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4359818353600928E-6</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15165,11 +15165,11 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16628940577952522</v>
+        <v>0.17495031233054217</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.4108185211517183</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15177,39 +15177,39 @@
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63867534411971372</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62984902599283954</v>
+        <v>0.68288894397118394</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58300460659062048</v>
+        <v>0.59454925226568223</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44304411192440885</v>
+        <v>0.47044890235272285</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25763661825446632</v>
+        <v>0.26011389342999003</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5760681350796724E-2</v>
+        <v>5.740070139052604E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5161673859693715E-4</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.9446352957399832E-5</v>
+        <v>5.8220654958278186E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.6645560939928683E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5389344262295074E-6</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.3314437231416288E-6</v>
+        <v>5.2791746670323972E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3938020611031058E-3</v>
+        <v>8.1394444228878593E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16628940577952522</v>
+        <v>0.16802158708972861</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.42775949109611905</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57304500346840825</v>
+        <v>0.55602386475152488</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60705775282665864</v>
+        <v>0.62602830760249173</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68951893371847706</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55991531524049687</v>
+        <v>0.57145996091555862</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45674650713856585</v>
+        <v>0.44304411192440885</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24277296720132402</v>
+        <v>0.26011389342999003</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6854028043949602E-2</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6568140814081463E-4</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>5.9446352957399832E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5514309225564595E-5</v>
+        <v>1.5675916613330893E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17001,7 +17001,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3536639344262295E-5</v>
+        <v>2.2152131147540982E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3040084118131113E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,55 +26485,55 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1353214580087234E-2</v>
+        <v>2.156463254622671E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42842557133717324</v>
+        <v>0.45028401885437597</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0894810154912453</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4243568924129162</v>
+        <v>1.3807541304002759</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.614955400993271</v>
+        <v>1.5350071138153862</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6674890961468525</v>
+        <v>1.6338024477398454</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4303824329483521</v>
+        <v>1.4893672755441603</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0907755352682578</v>
+        <v>1.1022573830079236</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62096926866045088</v>
+        <v>0.65201773209347347</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14164852110572923</v>
+        <v>0.14025981011449659</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0439290724921126E-4</v>
+        <v>8.9561239358659751E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4887619456889457E-4</v>
+        <v>1.5489139434945597E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9891167596232968E-5</v>
+        <v>3.8717897961049643E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,27 +26558,27 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3138099389398654</v>
+        <v>2.2911255277737883</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.915254840102304</v>
+        <v>1.9551559826044351</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9844672154298235</v>
+        <v>2.0471346011802392</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1130643485212461</v>
+        <v>1.9118201248525559</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7940048670448951</v>
+        <v>1.7229551693401468</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5541689479249494</v>
+        <v>1.5858866815560706</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26586,27 +26586,27 @@
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2802358118383304</v>
+        <v>1.2418287374831802</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1258137109738111</v>
+        <v>1.2087684054666183</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676188156174111</v>
+        <v>1.0894069547116441</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0538919566191796</v>
+        <v>1.1204535538793383</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0178496549148142</v>
+        <v>1.0499922755963347</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.98916529189293634</v>
+        <v>1.0491147035228112</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26614,43 +26614,43 @@
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1814795409323788</v>
+        <v>1.2685359281589754</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4368075104182534</v>
+        <v>1.4089083354586758</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3480781201289271</v>
+        <v>1.4744604438910143</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5385310442936277</v>
+        <v>1.665420202585886</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4636141983324147</v>
+        <v>1.4937918106691654</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5745720770466822</v>
+        <v>1.5430806355057487</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6596189589780561</v>
+        <v>1.7114820514461202</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7634634671189149</v>
+        <v>1.7466685769558774</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7119201346516064</v>
+        <v>1.6460770525496216</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8446017140329807</v>
+        <v>1.8259693734871931</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1883695355191256E-5</v>
+        <v>1.1191441256830601E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5859010697631888E-6</v>
+        <v>6.7834781018560848E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,55 +26687,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0465189323904138E-2</v>
+        <v>1.0042353391625182E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22295616467546772</v>
+        <v>0.21858447517202717</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51777315587702744</v>
+        <v>0.56631438924049882</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69037706520013797</v>
+        <v>0.75578120821909844</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80747770049663548</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82532288597167447</v>
+        <v>0.85058787227692978</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72256432179865204</v>
+        <v>0.70781811114969995</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5798333108531265</v>
+        <v>0.60279700633245825</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30117009530031869</v>
+        <v>0.31048463433022544</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.9435549561631976E-2</v>
+        <v>7.1518616048480935E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3024516946807136E-4</v>
+        <v>4.4341593996199193E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2934297339306934E-5</v>
+        <v>7.8197597147298159E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9358948980524821E-5</v>
+        <v>1.8772314162933162E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2114446721311475E-5</v>
+        <v>1.1999071038251367E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.6517600804608211E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,7 +26788,7 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0148062374694922E-2</v>
+        <v>1.0042353391625182E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26796,47 +26796,47 @@
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53934703737190359</v>
+        <v>0.51237968550330837</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.71217844620645809</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83945701536778938</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84216621017517801</v>
+        <v>0.80847956176817082</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75942984842103223</v>
+        <v>0.71519121647417605</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5798333108531265</v>
+        <v>0.59131515859279238</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29806524895701642</v>
+        <v>0.29496040261371415</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0129905057248296E-2</v>
+        <v>6.8741194066015657E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.2585491263676448E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.8197597147298159E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9945583798116484E-5</v>
+        <v>2.0336673676510925E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26869,7 +26869,7 @@
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5200420590655566E-6</v>
+        <v>6.4541830483679252E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,15 +26889,15 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.025377135776466E-2</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21202694091686636</v>
+        <v>0.21858447517202717</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55013397811934173</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26905,15 +26905,15 @@
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82346735793221248</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86743119648043332</v>
+        <v>0.80005789966641905</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.77417605906998432</v>
+        <v>0.72993742712312815</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26921,23 +26921,23 @@
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30117009530031869</v>
+        <v>0.31048463433022544</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1518616048480935E-2</v>
+        <v>6.8741194066015657E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1707439897415078E-4</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3686197311877109E-5</v>
+        <v>7.4438097284447284E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9163404041327603E-5</v>
+        <v>2.0532218615708147E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.284438524590164E-5</v>
+        <v>2.3075136612021857E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3435238182316905E-5</v>
+        <v>1.3303520160921642E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,11 +27240,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0296124749389844E-2</v>
+        <v>2.2198886444645145E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43279726084061382</v>
+        <v>0.43716895034405434</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27252,19 +27252,19 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3952883844044894</v>
+        <v>1.3807541304002759</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5509967712509631</v>
+        <v>1.5190174563798093</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6674890961468525</v>
+        <v>1.7517057171643704</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4746210648952083</v>
+        <v>1.4451286435973041</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27272,23 +27272,23 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64580803940686893</v>
+        <v>0.6085498832872418</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13470496614956604</v>
+        <v>0.13192754416710076</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.6049033893614271E-4</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4737239462375422E-4</v>
+        <v>1.5338759440431562E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8717897961049643E-5</v>
+        <v>3.7544628325866324E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,99 +27313,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3138099389398654</v>
+        <v>2.2911255277737883</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.094809981361895</v>
+        <v>1.9551559826044351</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1306911155141264</v>
+        <v>1.9844672154298235</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.072815503787508</v>
+        <v>2.0325666590537699</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7584800181925211</v>
+        <v>1.7051927449139597</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6651810156338742</v>
+        <v>1.57002781474051</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4696339308265798</v>
+        <v>1.3697558966927346</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2162240212464137</v>
+        <v>1.3442476024302468</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1376643816156409</v>
+        <v>1.1495150522574702</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676188156174111</v>
+        <v>1.111195093805877</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1648279520527773</v>
+        <v>1.1426407529660578</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.071420689384015</v>
+        <v>1.0499922755963347</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95919058607799879</v>
+        <v>0.94919901747301971</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0229183862572979</v>
+        <v>1.0330462910717266</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1939161676790355</v>
+        <v>1.2312260479190054</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.394958747978887</v>
+        <v>1.4368075104182534</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.390205561382956</v>
+        <v>1.4463754830549949</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5226698995070955</v>
+        <v>1.5861144786532246</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4937918106691654</v>
+        <v>1.4334365859956639</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115891939648149</v>
+        <v>1.6375549601285497</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.728769748935475</v>
+        <v>1.6423312614887011</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7298736867928401</v>
+        <v>1.5955145654885416</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5802339704476367</v>
+        <v>1.5637731999221405</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8259693734871931</v>
+        <v>1.9377634167619193</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,11 +27418,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.130681693989071E-5</v>
+        <v>1.1768319672131148E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3224650269726606E-6</v>
+        <v>6.9151961232513485E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,15 +27442,15 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0570898306973877E-2</v>
+        <v>1.0888025256183095E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.20765525141342581</v>
+        <v>0.22951369893062853</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53395356699818453</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27458,39 +27458,39 @@
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82346735793221248</v>
+        <v>0.77549838562548157</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85900953437868155</v>
+        <v>0.83374454807342624</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71519121647417605</v>
+        <v>0.72256432179865204</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5798333108531265</v>
+        <v>0.59131515859279238</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31669432701682998</v>
+        <v>0.31358948067352771</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2212971544097254E-2</v>
+        <v>6.5963772083550379E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1707439897415078E-4</v>
+        <v>4.3463542629937818E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.5941897229587634E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>2.0532218615708147E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,11 +27519,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1999071038251367E-5</v>
+        <v>1.1652943989071037E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27547,51 +27547,51 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22077031992374743</v>
+        <v>0.20984109616514607</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51777315587702744</v>
+        <v>0.53934703737190359</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73397982721277832</v>
+        <v>0.74124695421488507</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83945701536778938</v>
+        <v>0.78349321434327002</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83374454807342624</v>
+        <v>0.80847956176817082</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70044500582522395</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55112869150396182</v>
+        <v>0.56261053924362769</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31669432701682998</v>
+        <v>0.30117009530031869</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1518616048480935E-2</v>
+        <v>6.8046838570399337E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.4780619679329875E-4</v>
+        <v>4.5219645362460563E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3686197311877109E-5</v>
+        <v>7.2182397366736759E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>1.9750038858919265E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1076065573770491E-5</v>
+        <v>1.1999071038251367E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.849337112553717E-6</v>
+        <v>6.6517600804608211E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,55 +27644,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.025377135776466E-2</v>
+        <v>1.0570898306973877E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22077031992374743</v>
+        <v>0.21421278566858662</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55552744849306068</v>
+        <v>0.53395356699818453</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.7485140812169917</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83945701536778938</v>
+        <v>0.77549838562548157</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85058787227692978</v>
+        <v>0.8169012238699227</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76680295374550833</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60279700633245825</v>
+        <v>0.57409238698329357</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29806524895701642</v>
+        <v>0.32600886604673673</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7352483074783018E-2</v>
+        <v>7.2907327039713574E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1707439897415078E-4</v>
+        <v>4.2585491263676448E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5189997257017459E-5</v>
+        <v>7.8949497119868334E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9358948980524821E-5</v>
+        <v>1.9554493919722043E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2382882513661202E-5</v>
+        <v>2.3536639344262295E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3171802139526378E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,39 +27914,39 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1353214580087234E-2</v>
+        <v>2.0296124749389844E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45465570835781655</v>
+        <v>0.44154063984749486</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.046333252501493</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4243568924129162</v>
+        <v>1.5115624164381969</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6309450584288481</v>
+        <v>1.56698642868654</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7685490413678739</v>
+        <v>1.7517057171643704</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4303824329483521</v>
+        <v>1.5483521181399686</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1941121649252506</v>
+        <v>1.1137392307475895</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64580803940686893</v>
+        <v>0.58992080522742829</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27954,15 +27954,15 @@
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.5170982527352896E-4</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5639519429459632E-4</v>
+        <v>1.5789899423973667E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9108987839444087E-5</v>
+        <v>3.715353844747188E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,99 +27987,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2003878831094799</v>
+        <v>2.3364943501059425</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.915254840102304</v>
+        <v>1.9352054113533694</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0262454725967673</v>
+        <v>2.1515802440975982</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9118201248525559</v>
+        <v>2.0526910814206394</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7940048670448951</v>
+        <v>1.8650545647496437</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5224512142938278</v>
+        <v>1.6334632820027528</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3840241872832837</v>
+        <v>1.3697558966927346</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2930381699567137</v>
+        <v>1.3314452443118636</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.185067064182959</v>
+        <v>1.2206190761084481</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0349366069760619</v>
+        <v>1.1329832329001097</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0538919566191796</v>
+        <v>1.1648279520527773</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1035633100655355</v>
+        <v>1.071420689384015</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0091484291028947</v>
+        <v>0.94919901747301971</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0533021007005841</v>
+        <v>1.0127904814428692</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1814795409323788</v>
+        <v>1.3058458083989453</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.394958747978887</v>
+        <v>1.4228579229384648</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3761630809649468</v>
+        <v>1.3621206005469368</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5861144786532246</v>
+        <v>1.5702533338666924</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4485253921640393</v>
+        <v>1.508880616837541</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6375549601285497</v>
+        <v>1.5115891939648149</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7633451439141845</v>
+        <v>1.7806328414035395</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6626941261406909</v>
+        <v>1.6291043458146162</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6625378230751178</v>
+        <v>1.6460770525496216</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9377634167619193</v>
+        <v>1.8632340545787685</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1768319672131148E-5</v>
+        <v>1.1537568306010929E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.5859010697631888E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,7 +28116,7 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.03594803408344E-2</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28124,47 +28124,47 @@
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5231666262507465</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69037706520013797</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82346735793221248</v>
+        <v>0.78349321434327002</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83374454807342624</v>
+        <v>0.88427452068393697</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70044500582522395</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55112869150396182</v>
+        <v>0.55686961537379476</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32600886604673673</v>
+        <v>0.29496040261371415</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6658127579166698E-2</v>
+        <v>7.2212971544097254E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5658671045591245E-4</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1430497394166584E-5</v>
+        <v>7.5189997257017459E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9163404041327603E-5</v>
+        <v>2.0532218615708147E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2114446721311475E-5</v>
+        <v>1.1191441256830601E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5859010697631888E-6</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,11 +28217,11 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0148062374694922E-2</v>
+        <v>1.0676607290043617E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22077031992374743</v>
+        <v>0.22295616467546772</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28229,15 +28229,15 @@
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72671270021067158</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.76750355690769312</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85900953437868155</v>
+        <v>0.84216621017517801</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28245,23 +28245,23 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58557423472295944</v>
+        <v>0.56261053924362769</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32290401970343446</v>
+        <v>0.3042749416436209</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2907327039713574E-2</v>
+        <v>6.5963772083550379E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2585491263676448E-4</v>
+        <v>4.3463542629937818E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1430497394166584E-5</v>
+        <v>7.6693797202157809E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1537568306010929E-5</v>
+        <v>1.1076065573770491E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.9151961232513485E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,7 +28318,7 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0148062374694922E-2</v>
+        <v>1.0570898306973877E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28326,31 +28326,31 @@
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51777315587702744</v>
+        <v>0.56092091886677975</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69037706520013797</v>
+        <v>0.69764419220224472</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83945701536778938</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82532288597167447</v>
+        <v>0.88427452068393697</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76680295374550833</v>
+        <v>0.75205674309655623</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54538776763412888</v>
+        <v>0.57409238698329357</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29496040261371415</v>
+        <v>0.31358948067352771</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28358,15 +28358,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1707439897415078E-4</v>
+        <v>4.3463542629937818E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5941897229587634E-5</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0141128737313706E-5</v>
+        <v>2.0532218615708147E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>

<commit_message>
ADN node 5. Flex growth modified
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
+++ b/data/IEEE9/ieee18_1/ieee18_1_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56600F21-090D-44D3-8422-9DC383D50D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E4CAEE-A4E7-4BC6-97FE-AE088216C18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8355" yWindow="4620" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26250" yWindow="4200" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -249,12 +249,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.01</v>
+            <v>1.4999999999999999E-2</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.1</v>
+            <v>7.4999999999999997E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -7724,18 +7724,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
       <sheetData sheetId="27">
         <row r="2">
           <cell r="B2">
@@ -8898,8 +8898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.7442622950819669E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0349273109627868E-5</v>
+        <v>1.0140196885190942E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,11 +13510,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.6787604122206212E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35682934990189791</v>
+        <v>0.36029371252230469</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13526,19 +13526,19 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2267625421705393</v>
+        <v>1.3279388343083158</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2596980519856791</v>
+        <v>1.3392579289531956</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1890985045313645</v>
+        <v>1.1198306304809937</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.93176287456267437</v>
+        <v>0.90435808413436036</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13546,19 +13546,19 @@
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11042801600844057</v>
+        <v>0.10933466931528769</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6807180333418054E-4</v>
+        <v>7.1729814673775183E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2869828990777284E-4</v>
+        <v>1.1766700791567802E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2967907104324765E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,15 +13583,15 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1804043572288254</v>
+        <v>3.1192427349744243</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8077543078660447</v>
+        <v>2.8633534030713133</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7285456935130408</v>
+        <v>2.6194038657725196</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13599,7 +13599,7 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3209567916884448</v>
+        <v>2.2972735591201952</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13607,71 +13607,71 @@
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8002359356040025</v>
+        <v>1.8369754444938802</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5668551567693678</v>
+        <v>1.6493212176519663</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6793562815281096</v>
+        <v>1.5824703422091801</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5041017740523399</v>
+        <v>1.430371294932127</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4788862363948292</v>
+        <v>1.4643873517242918</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5025643199579823</v>
+        <v>1.4158779168834834</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3257307195545065</v>
+        <v>1.3527864485250065</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3329487730123768</v>
+        <v>1.3062897975521293</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7460497808471001</v>
+        <v>1.6956829602457413</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9061874785840249</v>
+        <v>1.8874993660488877</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.031179519378032</v>
+        <v>2.0116489470763197</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0754083080268786</v>
+        <v>2.1186459811107721</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9939091355001093</v>
+        <v>2.0350206640671216</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0822151193029104</v>
+        <v>2.0401501673978011</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1462034119843834</v>
+        <v>2.3232098789521678</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3839255580606258</v>
+        <v>2.2249971875232504</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2190691637693529</v>
+        <v>2.2630111274083502</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0846994535519115E-6</v>
+        <v>8.7213114754098344E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>4.965560330377007E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,31 +13712,31 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.902517337533597E-3</v>
+        <v>8.0546585434827789E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.18187903757135573</v>
+        <v>0.17841467495094895</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4447004610405198</v>
+        <v>0.41928900612391867</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57871871637403605</v>
+        <v>0.55035015184589708</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64499886237832482</v>
+        <v>0.61338127108526963</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68951893371847706</v>
+        <v>0.65636898498201179</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5656876380780278</v>
+        <v>0.54837066956543501</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13744,23 +13744,23 @@
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25515934307894261</v>
+        <v>0.2378184168502766</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4667334657643847E-2</v>
+        <v>5.357398796449097E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6216524075484527E-4</v>
+        <v>3.5161673859693715E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8220654958278186E-5</v>
+        <v>6.0059201956960658E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6968775715461277E-5</v>
+        <v>1.5999131388863491E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,11 +13789,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8121584699453533E-6</v>
+        <v>9.3572404371584697E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.2242303022929415E-3</v>
+        <v>8.8177314581285166E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17668249364074556</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.40234803617951792</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55035015184589708</v>
+        <v>0.54467643894026918</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61970478934388062</v>
+        <v>0.62602830760249173</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.66962896447659781</v>
+        <v>0.62984902599283954</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57723228375308955</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.46131397220995152</v>
+        <v>0.43390918178163751</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.25763661825446632</v>
+        <v>0.24029569202580031</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5214008004220286E-2</v>
+        <v>5.4120661311067408E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.481005712109678E-4</v>
+        <v>3.6568140814081463E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.3123446954764769E-5</v>
+        <v>5.9446352957399832E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5675916613330893E-5</v>
+        <v>1.5999131388863491E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.0846994535519115E-6</v>
+        <v>8.6304644808743156E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>4.965560330377007E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,55 +13914,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.902517337533597E-3</v>
+        <v>8.8177314581285166E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17841467495094895</v>
+        <v>0.16455722446932183</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4447004610405198</v>
+        <v>0.42352424861001886</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55602386475152488</v>
+        <v>0.53900272603464139</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63867534411971372</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.64310900548742567</v>
+        <v>0.69614892346577006</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59454925226568223</v>
+        <v>0.55414299240296594</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.47958383249549419</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24772751755237146</v>
+        <v>0.25763661825446632</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6307354697373163E-2</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.481005712109678E-4</v>
+        <v>3.5161673859693715E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.0672050956521478E-5</v>
+        <v>6.1284899956082304E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5837524001097193E-5</v>
+        <v>1.6645560939928683E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,11 +14160,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0349273109627868E-5</v>
+        <v>1.0140196885190942E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14184,51 +14184,51 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7296319398636704E-2</v>
+        <v>1.6278888845775719E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34643626204067757</v>
+        <v>0.34297189942027079</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81316655733123622</v>
+        <v>0.82163704230343659</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1120477295030498</v>
+        <v>1.0780054520692828</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2141155056533173</v>
+        <v>1.2267625421705393</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3259979494586096</v>
+        <v>1.2862180109748513</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1429199218311172</v>
+        <v>1.2121877958814882</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88608822384881769</v>
+        <v>0.89522315399158903</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.51527323650893264</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10824132262213482</v>
+        <v>0.10714797592898194</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2433048150969054E-4</v>
+        <v>7.0323347719387431E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2379549791128626E-4</v>
+        <v>1.2134410191304296E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,11 +14257,11 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.905177057084023</v>
+        <v>3.1804043572288254</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8077543078660447</v>
+        <v>2.7521552126607762</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14269,19 +14269,19 @@
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8168325671109375</v>
+        <v>2.7074410111066287</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4393729545296923</v>
+        <v>2.3920064893931934</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1321132982057289</v>
+        <v>2.1948225128588388</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.855345198938819</v>
+        <v>1.9288242167185743</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14289,67 +14289,67 @@
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6470609684217996</v>
+        <v>1.6793562815281096</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5041017740523399</v>
+        <v>1.430371294932127</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5078840057359042</v>
+        <v>1.4788862363948292</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3725347153462339</v>
+        <v>1.3869824491919835</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.406897906466007</v>
+        <v>1.4204257709512569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.266301334361758</v>
+        <v>1.3462782607425006</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6285271994439297</v>
+        <v>1.6117382592434768</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8874993660488877</v>
+        <v>1.7753706908380624</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9530572301711844</v>
+        <v>1.8749349409643368</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1186459811107721</v>
+        <v>2.2267401638205051</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0555764283506281</v>
+        <v>2.0350206640671216</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1663450231131289</v>
+        <v>2.1873774990656836</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1240776036134101</v>
+        <v>2.1462034119843834</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2249971875232504</v>
+        <v>2.3839255580606258</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2630111274083502</v>
+        <v>2.1092142546718602</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4580498551852976</v>
+        <v>2.4083922823532715</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9938524590163926E-6</v>
+        <v>8.6304644808743156E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>5.3837127792508603E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,15 +14386,15 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3090161816980236E-3</v>
+        <v>8.4785879405081879E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17495031233054217</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.44046521855441961</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14402,27 +14402,27 @@
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60073423456804753</v>
+        <v>0.65764589889554681</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.67625895422389093</v>
+        <v>0.69614892346577006</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60609389794074409</v>
+        <v>0.5887769294281513</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44304411192440885</v>
+        <v>0.47501636742410852</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.24277296720132402</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5760681350796724E-2</v>
+        <v>5.1933967924761654E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14430,11 +14430,11 @@
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>6.3736295954325596E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5514309225564595E-5</v>
+        <v>1.5837524001097193E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,7 +14463,7 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9938524590163926E-6</v>
+        <v>8.9030054644808738E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14491,51 +14491,51 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16455722446932183</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42352424861001886</v>
+        <v>0.4108185211517183</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59573985509091953</v>
+        <v>0.59006614218529174</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60073423456804753</v>
+        <v>0.64499886237832482</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62984902599283954</v>
+        <v>0.6629989747293048</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.58300460659062048</v>
+        <v>0.57145996091555862</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44761157699579451</v>
+        <v>0.47044890235272285</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.2378184168502766</v>
+        <v>0.24029569202580031</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2480641271338092E-2</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4458440382499839E-4</v>
+        <v>3.3403590166709027E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.8833503957839012E-5</v>
+        <v>6.3123446954764769E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6968775715461277E-5</v>
+        <v>1.6160738776629788E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,11 +14564,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5389344262295074E-6</v>
+        <v>9.1755464480874303E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4359818353600928E-6</v>
+        <v>5.1223674987047025E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,27 +14588,27 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3938020611031058E-3</v>
+        <v>8.4785879405081879E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.169753768399932</v>
+        <v>0.18014685626115234</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43622997606831942</v>
+        <v>0.41928900612391867</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54467643894026918</v>
+        <v>0.56169757765715267</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61970478934388062</v>
+        <v>0.64499886237832482</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6629989747293048</v>
+        <v>0.64973899523471867</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14620,23 +14620,23 @@
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24277296720132402</v>
+        <v>0.25515934307894261</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.4120661311067408E-2</v>
+        <v>5.5214008004220286E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.6919757552678404E-4</v>
+        <v>3.481005712109678E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4349144953886422E-5</v>
+        <v>6.3123446954764769E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6483953552162382E-5</v>
+        <v>1.5675916613330893E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8532786885245898E-5</v>
+        <v>1.8714480874316939E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0035658772972477E-5</v>
+        <v>1.0140196885190942E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,27 +14858,27 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6109317086965558E-2</v>
+        <v>1.7465891157446869E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.32911444893864367</v>
+        <v>0.34297189942027079</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8555189821922381</v>
+        <v>0.83857801224783735</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1574374327480721</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2647036517222054</v>
+        <v>1.2899977247566496</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2862180109748513</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14890,23 +14890,23 @@
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47563683370055321</v>
+        <v>0.48059138405160062</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11152136270159345</v>
+        <v>0.10933466931528769</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3136281628162925E-4</v>
+        <v>6.962011424219356E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2624689390952954E-4</v>
+        <v>1.2502119591040791E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0705403675596596E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,39 +14931,39 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9357578682112226</v>
+        <v>3.1498235461016248</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8911529506739471</v>
+        <v>2.6687565698528743</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.783116607383302</v>
+        <v>2.7285456935130408</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7347889001077057</v>
+        <v>2.5980494551023203</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3209567916884448</v>
+        <v>2.2499070939836967</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1739194413078025</v>
+        <v>2.1112102266546926</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9288242167185743</v>
+        <v>1.9104544622736355</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6328280054754465</v>
+        <v>1.7152940663580449</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5501750291028702</v>
+        <v>1.5663226856560251</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14971,39 +14971,39 @@
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.449888467053754</v>
+        <v>1.3773940437010661</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.430325650729233</v>
+        <v>1.4736688522664827</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4204257709512569</v>
+        <v>1.3933700419807569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3862667239328719</v>
+        <v>1.319619285282253</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7124719004461941</v>
+        <v>1.6621050798448356</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7753706908380624</v>
+        <v>1.8314350284434751</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0116489470763197</v>
+        <v>2.0507100916797434</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1402648176527186</v>
+        <v>2.1186459811107721</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0966879569176409</v>
+        <v>2.117243721201147</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15011,19 +15011,19 @@
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1683292203553566</v>
+        <v>2.1240776036134101</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3385174521928045</v>
+        <v>2.2931093463249828</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1092142546718602</v>
+        <v>2.2190691637693529</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4580498551852976</v>
+        <v>2.4083922823532715</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.1755464480874303E-6</v>
+        <v>8.6304644808743156E-6</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2269056109231657E-6</v>
+        <v>5.0178293864862386E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,55 +15060,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.0546585434827789E-3</v>
+        <v>8.1394444228878593E-3</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17148594971013539</v>
+        <v>0.16628940577952522</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.41505376363781848</v>
+        <v>0.43199473358221924</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.54467643894026918</v>
+        <v>0.55035015184589708</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61338127108526963</v>
+        <v>0.66396941715415791</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62984902599283954</v>
+        <v>0.67625895422389093</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57723228375308955</v>
+        <v>0.60032157510321316</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47501636742410852</v>
+        <v>0.45217904206718018</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.24277296720132402</v>
+        <v>0.25763661825446632</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.6854028043949602E-2</v>
+        <v>5.4667334657643847E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5161673859693715E-4</v>
+        <v>3.6216524075484527E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2510597955203957E-5</v>
+        <v>5.8833503957839012E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5352701837798298E-5</v>
+        <v>1.5514309225564595E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,7 +15137,7 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9030054644808738E-6</v>
+        <v>9.4480874316939885E-6</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,47 +15161,47 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.1394444228878593E-3</v>
+        <v>8.2242303022929415E-3</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.17495031233054217</v>
+        <v>0.18014685626115234</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.4108185211517183</v>
+        <v>0.43622997606831942</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56169757765715267</v>
+        <v>0.56737129056278046</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65764589889554681</v>
+        <v>0.60705775282665864</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.68288894397118394</v>
+        <v>0.63647901574013255</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59454925226568223</v>
+        <v>0.5887769294281513</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47044890235272285</v>
+        <v>0.46588143728133719</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.23534114167475287</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.740070139052604E-2</v>
+        <v>5.5760681350796724E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.481005712109678E-4</v>
+        <v>3.5513290598290651E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15209,7 +15209,7 @@
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6645560939928683E-5</v>
+        <v>1.6322346164396085E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.7213114754098344E-6</v>
+        <v>9.4480874316939885E-6</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.2791746670323972E-6</v>
+        <v>5.4359818353600928E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,15 +15262,15 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.1394444228878593E-3</v>
+        <v>8.3090161816980236E-3</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.16802158708972861</v>
+        <v>0.17495031233054217</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42775949109611905</v>
+        <v>0.43199473358221924</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15278,11 +15278,11 @@
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62602830760249173</v>
+        <v>0.66396941715415791</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65636898498201179</v>
+        <v>0.6629989747293048</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15290,19 +15290,19 @@
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44304411192440885</v>
+        <v>0.46588143728133719</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26011389342999003</v>
+        <v>0.24525024237684775</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5214008004220286E-2</v>
+        <v>5.357398796449097E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5513290598290651E-4</v>
+        <v>3.4458440382499839E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17000,7 +17000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303073B7-556E-4714-A27A-3E87EB1A31BB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2152131147540982E-5</v>
+        <v>2.3998142076502733E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2644930053945321E-5</v>
+        <v>1.3698674225107434E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,11 +26485,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.1987468478505665E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45028401885437597</v>
+        <v>0.45465570835781655</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26497,43 +26497,43 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3807541304002759</v>
+        <v>1.3952883844044894</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5350071138153862</v>
+        <v>1.6789140307355788</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.6674890961468525</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4893672755441603</v>
+        <v>1.4598748542462563</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1022573830079236</v>
+        <v>1.1481847739665871</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65201773209347347</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14025981011449659</v>
+        <v>0.13470496614956604</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9561239358659751E-4</v>
+        <v>8.3414879794830156E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5489139434945597E-4</v>
+        <v>1.5639519429459632E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8717897961049643E-5</v>
+        <v>3.9108987839444087E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,87 +26558,87 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2911255277737883</v>
+        <v>2.3364943501059425</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9551559826044351</v>
+        <v>1.895304268851238</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0471346011802392</v>
+        <v>2.0053563440132955</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9118201248525559</v>
+        <v>2.0929399261543771</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7229551693401468</v>
+        <v>1.7940048670448951</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5858866815560706</v>
+        <v>1.5065923474782672</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3840241872832837</v>
+        <v>1.4696339308265798</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2418287374831802</v>
+        <v>1.3442476024302468</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2087684054666183</v>
+        <v>1.1732163935411295</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0894069547116441</v>
+        <v>1.1220891633529932</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1204535538793383</v>
+        <v>1.1648279520527773</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0499922755963347</v>
+        <v>1.1035633100655355</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0491147035228112</v>
+        <v>0.99915686049791552</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.97227886218515425</v>
+        <v>1.0330462910717266</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2685359281589754</v>
+        <v>1.2312260479190054</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4089083354586758</v>
+        <v>1.3670595730193091</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4744604438910143</v>
+        <v>1.404248041800966</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.665420202585886</v>
+        <v>1.6336979130128215</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4937918106691654</v>
+        <v>1.5843246476794182</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5430806355057487</v>
+        <v>1.6375549601285497</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7114820514461202</v>
+        <v>1.7633451439141845</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26646,11 +26646,11 @@
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6460770525496216</v>
+        <v>1.7119201346516064</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8259693734871931</v>
+        <v>1.8446017140329807</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1191441256830601E-5</v>
+        <v>1.1999071038251367E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7834781018560848E-6</v>
+        <v>6.3224650269726606E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26687,43 +26687,43 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0042353391625182E-2</v>
+        <v>1.0782316273113355E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21858447517202717</v>
+        <v>0.21202694091686636</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56631438924049882</v>
+        <v>0.51237968550330837</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75578120821909844</v>
+        <v>0.74124695421488507</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.83146218665000093</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.85058787227692978</v>
+        <v>0.8758528585821852</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70781811114969995</v>
+        <v>0.77417605906998432</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60279700633245825</v>
+        <v>0.59705608246262531</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31048463433022544</v>
+        <v>0.30737978798692317</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1518616048480935E-2</v>
+        <v>6.6658127579166698E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26735,7 +26735,7 @@
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8772314162933162E-5</v>
+        <v>1.9554493919722043E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1999071038251367E-5</v>
+        <v>1.130681693989071E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6517600804608211E-6</v>
+        <v>6.9151961232513485E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,7 +26788,7 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0042353391625182E-2</v>
+        <v>1.0993734239252833E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26796,47 +26796,47 @@
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51237968550330837</v>
+        <v>0.51777315587702744</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71217844620645809</v>
+        <v>0.7485140812169917</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.82346735793221248</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80847956176817082</v>
+        <v>0.86743119648043332</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.71519121647417605</v>
+        <v>0.74468363777208013</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59131515859279238</v>
+        <v>0.58557423472295944</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29496040261371415</v>
+        <v>0.32600886604673673</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.8741194066015657E-2</v>
+        <v>6.8046838570399337E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2585491263676448E-4</v>
+        <v>4.4780619679329875E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1430497394166584E-5</v>
+        <v>7.5189997257017459E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0336673676510925E-5</v>
+        <v>1.8967859102130381E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1191441256830601E-5</v>
+        <v>1.2114446721311475E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.4541830483679252E-6</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,27 +26889,27 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.1099443222322572E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21858447517202717</v>
+        <v>0.22514200942718798</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51777315587702744</v>
+        <v>0.51237968550330837</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.76304833522120519</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83945701536778938</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.80005789966641905</v>
+        <v>0.85058787227692978</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26917,11 +26917,11 @@
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56835146311346063</v>
+        <v>0.59131515859279238</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31048463433022544</v>
+        <v>0.3042749416436209</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26929,15 +26929,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2146465580545766E-4</v>
+        <v>4.5658671045591245E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.4438097284447284E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0532218615708147E-5</v>
+        <v>2.0141128737313706E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27216,11 +27216,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3075136612021857E-5</v>
+        <v>2.261363387978142E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3303520160921642E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,11 +27240,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2198886444645145E-2</v>
+        <v>2.0084706783250365E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43716895034405434</v>
+        <v>0.41968219233029214</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27252,11 +27252,11 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3807541304002759</v>
+        <v>1.4098226384087029</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5190174563798093</v>
+        <v>1.5509967712509631</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27264,31 +27264,31 @@
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4451286435973041</v>
+        <v>1.5336059074910167</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1711484694459189</v>
+        <v>1.0907755352682578</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.6085498832872418</v>
+        <v>0.58992080522742829</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13192754416710076</v>
+        <v>0.14303723209696187</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3414879794830156E-4</v>
+        <v>9.0439290724921126E-4</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5338759440431562E-4</v>
+        <v>1.5639519429459632E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7544628325866324E-5</v>
+        <v>3.8717897961049643E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,7 +27313,7 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2911255277737883</v>
+        <v>2.2003878831094799</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27321,23 +27321,23 @@
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9844672154298235</v>
+        <v>2.0471346011802392</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0325666590537699</v>
+        <v>2.0124422366869013</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7051927449139597</v>
+        <v>1.7584800181925211</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.57002781474051</v>
+        <v>1.6651810156338742</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3697558966927346</v>
+        <v>1.4268290590549317</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27345,67 +27345,67 @@
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1495150522574702</v>
+        <v>1.1969177348247888</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.111195093805877</v>
+        <v>1.0676188156174111</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1426407529660578</v>
+        <v>1.1093599543359784</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0499922755963347</v>
+        <v>1.071420689384015</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94919901747301971</v>
+        <v>0.96918215468297808</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0330462910717266</v>
+        <v>1.0533021007005841</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2312260479190054</v>
+        <v>1.2685359281589754</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4368075104182534</v>
+        <v>1.3391603980597313</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4463754830549949</v>
+        <v>1.3480781201289271</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5861144786532246</v>
+        <v>1.6336979130128215</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4334365859956639</v>
+        <v>1.4636141983324147</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6375549601285497</v>
+        <v>1.4958434731943482</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6423312614887011</v>
+        <v>1.797920538892894</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5955145654885416</v>
+        <v>1.7634634671189149</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5637731999221405</v>
+        <v>1.5966947409731327</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9377634167619193</v>
+        <v>1.9004987356703438</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,11 +27418,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1768319672131148E-5</v>
+        <v>1.1537568306010929E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.9151961232513485E-6</v>
+        <v>6.7176190911584525E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,55 +27442,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0888025256183095E-2</v>
+        <v>1.0993734239252833E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22951369893062853</v>
+        <v>0.22295616467546772</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55013397811934173</v>
+        <v>0.51237968550330837</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76304833522120519</v>
+        <v>0.73397982721277832</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.77549838562548157</v>
+        <v>0.75950872818990467</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83374454807342624</v>
+        <v>0.85900953437868155</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72256432179865204</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.59131515859279238</v>
+        <v>0.60279700633245825</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31358948067352771</v>
+        <v>0.3042749416436209</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5963772083550379E-2</v>
+        <v>6.8046838570399337E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3463542629937818E-4</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5941897229587634E-5</v>
+        <v>7.4438097284447284E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0532218615708147E-5</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27519,7 +27519,7 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1652943989071037E-5</v>
+        <v>1.1883695355191256E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,7 +27543,7 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.025377135776466E-2</v>
+        <v>1.0148062374694922E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27551,15 +27551,15 @@
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53934703737190359</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.74124695421488507</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78349321434327002</v>
+        <v>0.83146218665000093</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27571,27 +27571,27 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56261053924362769</v>
+        <v>0.55686961537379476</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.30117009530031869</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.8046838570399337E-2</v>
+        <v>7.0129905057248296E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.5219645362460563E-4</v>
+        <v>4.4780619679329875E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2182397366736759E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9750038858919265E-5</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,11 +27620,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1999071038251367E-5</v>
+        <v>1.130681693989071E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.6517600804608211E-6</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,35 +27644,35 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0570898306973877E-2</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21421278566858662</v>
+        <v>0.20984109616514607</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53395356699818453</v>
+        <v>0.55552744849306068</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.72671270021067158</v>
+        <v>0.70491131920435146</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.77549838562548157</v>
+        <v>0.83945701536778938</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8169012238699227</v>
+        <v>0.86743119648043332</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.73731053244760414</v>
+        <v>0.74468363777208013</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57409238698329357</v>
+        <v>0.56261053924362769</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27684,15 +27684,15 @@
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2585491263676448E-4</v>
+        <v>4.5658671045591245E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.8949497119868334E-5</v>
+        <v>7.6693797202157809E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9554493919722043E-5</v>
+        <v>1.9945583798116484E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3536639344262295E-5</v>
+        <v>2.422889344262295E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2644930053945321E-5</v>
+        <v>1.290836609673585E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,31 +27914,31 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0296124749389844E-2</v>
+        <v>2.0084706783250365E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44154063984749486</v>
+        <v>0.42842557133717324</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0247593710066167</v>
+        <v>1.0786940747438072</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115624164381969</v>
+        <v>1.4534254004213432</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.56698642868654</v>
+        <v>1.6629243733000019</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7517057171643704</v>
+        <v>1.6001157993328381</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5483521181399686</v>
+        <v>1.4598748542462563</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27950,7 +27950,7 @@
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13192754416710076</v>
+        <v>0.14303723209696187</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27958,11 +27958,11 @@
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5789899423973667E-4</v>
+        <v>1.5188379445917527E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.715353844747188E-5</v>
+        <v>3.9500077717838531E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27991,11 +27991,11 @@
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9352054113533694</v>
+        <v>2.0549088388597636</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1515802440975982</v>
+        <v>2.068023729763711</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28003,55 +28003,55 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8650545647496437</v>
+        <v>1.7584800181925211</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6334632820027528</v>
+        <v>1.5065923474782672</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3697558966927346</v>
+        <v>1.4981705120076785</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3314452443118636</v>
+        <v>1.2930381699567137</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2206190761084481</v>
+        <v>1.2324697467502774</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1329832329001097</v>
+        <v>1.1003010242587605</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1648279520527773</v>
+        <v>1.1426407529660578</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.071420689384015</v>
+        <v>1.0821348962778552</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94919901747301971</v>
+        <v>1.0491147035228112</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0127904814428692</v>
+        <v>1.0431741958861553</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3058458083989453</v>
+        <v>1.243662674665662</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4228579229384648</v>
+        <v>1.394958747978887</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3621206005469368</v>
+        <v>1.3480781201289271</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28059,27 +28059,27 @@
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.508880616837541</v>
+        <v>1.5239694230059164</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115891939648149</v>
+        <v>1.5273349147352819</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7806328414035395</v>
+        <v>1.6941943539567657</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6291043458146162</v>
+        <v>1.6962839064667656</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6460770525496216</v>
+        <v>1.5966947409731327</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8632340545787685</v>
+        <v>1.7700723518498298</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28092,11 +28092,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1537568306010929E-5</v>
+        <v>1.1883695355191256E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5859010697631888E-6</v>
+        <v>6.2566060162750292E-6</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28116,23 +28116,23 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0676607290043617E-2</v>
+        <v>1.0782316273113355E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.21858447517202717</v>
+        <v>0.22732785417890827</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55552744849306068</v>
+        <v>0.53395356699818453</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.72671270021067158</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.78349321434327002</v>
+        <v>0.79948287177884703</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28140,31 +28140,31 @@
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76680295374550833</v>
+        <v>0.73731053244760414</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.55686961537379476</v>
+        <v>0.57409238698329357</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.29496040261371415</v>
+        <v>0.31358948067352771</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2212971544097254E-2</v>
+        <v>7.2907327039713574E-2</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3902568313068505E-4</v>
+        <v>4.5219645362460563E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.5189997257017459E-5</v>
+        <v>7.2934297339306934E-5</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0532218615708147E-5</v>
+        <v>2.0336673676510925E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1191441256830601E-5</v>
+        <v>1.0960689890710382E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.2566060162750292E-6</v>
+        <v>6.5200420590655566E-6</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28221,51 +28221,51 @@
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22295616467546772</v>
+        <v>0.22077031992374743</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.53934703737190359</v>
+        <v>0.55013397811934173</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.70491131920435146</v>
+        <v>0.71217844620645809</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.76750355690769312</v>
+        <v>0.82346735793221248</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.84216621017517801</v>
+        <v>0.88427452068393697</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.77417605906998432</v>
+        <v>0.76680295374550833</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56261053924362769</v>
+        <v>0.56835146311346063</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.3042749416436209</v>
+        <v>0.31669432701682998</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.5963772083550379E-2</v>
+        <v>7.0129905057248296E-2</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3463542629937818E-4</v>
+        <v>4.3902568313068505E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.6693797202157809E-5</v>
+        <v>7.1430497394166584E-5</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0336673676510925E-5</v>
+        <v>1.8967859102130381E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1076065573770491E-5</v>
+        <v>1.1537568306010929E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.9151961232513485E-6</v>
+        <v>6.849337112553717E-6</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,55 +28318,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0570898306973877E-2</v>
+        <v>1.025377135776466E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.22514200942718798</v>
+        <v>0.20984109616514607</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.56092091886677975</v>
+        <v>0.52856009662446546</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.69764419220224472</v>
+        <v>0.75578120821909844</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.79948287177884703</v>
+        <v>0.78349321434327002</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.88427452068393697</v>
+        <v>0.8758528585821852</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.75205674309655623</v>
+        <v>0.75942984842103223</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.57409238698329357</v>
+        <v>0.55686961537379476</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.31358948067352771</v>
+        <v>0.29496040261371415</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.0129905057248296E-2</v>
+        <v>6.5963772083550379E-2</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3463542629937818E-4</v>
+        <v>4.2146465580545766E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.2934297339306934E-5</v>
+        <v>7.5189997257017459E-5</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0532218615708147E-5</v>
+        <v>1.857676922373594E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>